<commit_message>
deleted conflicting scripts from prior messy workflow.
</commit_message>
<xml_diff>
--- a/output_data/repo_catalogue.xlsx
+++ b/output_data/repo_catalogue.xlsx
@@ -515,7 +515,7 @@
     <t>2020-05-24 19:27:25</t>
   </si>
   <si>
-    <t>2020-05-29 21:26:38</t>
+    <t>2020-05-31 20:27:22</t>
   </si>
   <si>
     <t>2019-09-18 10:42:21</t>
@@ -605,7 +605,7 @@
     <t>2020-05-07 16:32:58</t>
   </si>
   <si>
-    <t>2020-05-29 21:26:35</t>
+    <t>2020-05-31 20:27:19</t>
   </si>
   <si>
     <t>Repository for the Data Science Campus Access to Services project (linked to datasciencecampus/graphite and datasciencecampus/propeR)</t>

</xml_diff>